<commit_message>
xlsx editor works fine for Name and Email
</commit_message>
<xml_diff>
--- a/src/Verification_Team_Roster.xlsx
+++ b/src/Verification_Team_Roster.xlsx
@@ -418,7 +418,18 @@
         </is>
       </c>
     </row>
-    <row r="4"/>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Nathan Weiler</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>nweiler@uoguelph.ca</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.9840277777777779" bottom="0.9840277777777779" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>